<commit_message>
added newml and webelement
</commit_message>
<xml_diff>
--- a/DataExcel/nopCommerce.xlsx
+++ b/DataExcel/nopCommerce.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>FirSTName</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>hfsc</t>
+  </si>
+  <si>
+    <t>situ</t>
+  </si>
+  <si>
+    <t>kumar</t>
+  </si>
+  <si>
+    <t>Babamama143</t>
   </si>
 </sst>
 </file>
@@ -401,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C1:C1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,6 +466,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>